<commit_message>
Finish the Problem 1 and 2
</commit_message>
<xml_diff>
--- a/data/Trash-Wheel-Collection-Totals-7-2020-2.xlsx
+++ b/data/Trash-Wheel-Collection-Totals-7-2020-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/730f13e1be2ad4cf/Documents/R file/P8105_R code/p8105_hw2_hz2770/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{BC254DC8-5C47-4102-B61F-BD7B5BA62AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DCA9A57-6C1C-449A-A3B8-5BDDFCC4D53A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{BC254DC8-5C47-4102-B61F-BD7B5BA62AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ADBA8F4-48B4-4489-ADD9-8EF243E6E909}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
@@ -1792,8 +1792,8 @@
       <xdr:rowOff>158214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>86546</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1333028</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1615379</xdr:rowOff>
     </xdr:to>
@@ -1837,7 +1837,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>856278</xdr:colOff>
+      <xdr:colOff>403546</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1863043</xdr:rowOff>
     </xdr:to>
@@ -2385,24 +2385,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DL547"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A522" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="M535" sqref="M535"/>
+      <selection pane="bottomLeft" sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="13.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.9140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.5" style="26" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="27"/>
   </cols>
@@ -33645,7 +33649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051BD652-3ACC-C74A-8467-89B1A58FDD59}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
@@ -35455,7 +35459,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:B15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>
@@ -35588,7 +35592,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="A1:XFD1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15"/>

</xml_diff>